<commit_message>
Added new cols to AE smaple uploads
</commit_message>
<xml_diff>
--- a/public/sample_uploads/account_entries_with_dup.xlsx
+++ b/public/sample_uploads/account_entries_with_dup.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD2DD54-4E3F-417B-804B-69B4EDAEAC3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{087F7501-0A34-4CC5-A3C2-84AEFD72CB45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -233,7 +233,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="29">
   <si>
     <t>Investor *</t>
   </si>
@@ -314,6 +314,12 @@
   </si>
   <si>
     <t>Amount (Folio Currency)</t>
+  </si>
+  <si>
+    <t>Parent Type</t>
+  </si>
+  <si>
+    <t>Parent Id</t>
   </si>
 </sst>
 </file>
@@ -747,10 +753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+      <selection activeCell="K1" sqref="K1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -766,7 +772,7 @@
     <col min="9" max="9" width="8.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -797,8 +803,14 @@
       <c r="J1" s="6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -826,7 +838,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
@@ -854,7 +866,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
@@ -884,7 +896,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
@@ -912,7 +924,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
@@ -940,7 +952,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -970,7 +982,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -998,7 +1010,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
@@ -1026,7 +1038,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
@@ -1054,7 +1066,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
@@ -1082,7 +1094,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
@@ -1110,7 +1122,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13" s="4" t="s">
         <v>7</v>
       </c>
@@ -1138,7 +1150,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
         <v>7</v>
       </c>
@@ -1166,7 +1178,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A15" s="4" t="s">
         <v>11</v>
       </c>
@@ -1194,7 +1206,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
         <v>14</v>
       </c>

</xml_diff>